<commit_message>
Cria Json consolidado e Salva em Excel
</commit_message>
<xml_diff>
--- a/arquivo_linkado.xlsx
+++ b/arquivo_linkado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Magal\Desktop\NEW_SAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CE05F3-7339-4670-9707-F16EBE78C545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C8D678-C599-40BC-B8DB-35BB1617E0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="135">
   <si>
     <t>Coluna extraída</t>
   </si>
@@ -381,28 +381,73 @@
   <si>
     <t>None</t>
   </si>
+  <si>
+    <t>twm_Fornecedor</t>
+  </si>
+  <si>
+    <t>twm_Identificador</t>
+  </si>
+  <si>
+    <t>twm_Categoria</t>
+  </si>
+  <si>
+    <t>twm_Subcategoria</t>
+  </si>
+  <si>
+    <t>twm_Data de emissão</t>
+  </si>
+  <si>
+    <t>twm_Localidade</t>
+  </si>
+  <si>
+    <t>twm_Status</t>
+  </si>
+  <si>
+    <t>twm_Metro Quadrado</t>
+  </si>
+  <si>
+    <t>twm_Nota fiscal</t>
+  </si>
+  <si>
+    <t>twm_Cód. Filial</t>
+  </si>
+  <si>
+    <t>twm_Alunos</t>
+  </si>
+  <si>
+    <t>twm_Mês</t>
+  </si>
+  <si>
+    <t>twm_Sigla</t>
+  </si>
+  <si>
+    <t>twm_AVB</t>
+  </si>
+  <si>
+    <t>twm_GRUPO</t>
+  </si>
+  <si>
+    <t>twm_Regional</t>
+  </si>
+  <si>
+    <t>twm_Divisional</t>
+  </si>
+  <si>
+    <t>twm_ES</t>
+  </si>
+  <si>
+    <t>twm_Concessionária</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -410,57 +455,19 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,30 +476,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF44546A"/>
-        <bgColor rgb="FF44546A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF44546A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -500,215 +489,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,11 +714,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V993"/>
+  <dimension ref="A1:V937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -936,76 +726,76 @@
     <col min="1" max="2" width="27.125" customWidth="1"/>
     <col min="3" max="3" width="33.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="27.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="35.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.125" style="2" customWidth="1"/>
     <col min="9" max="22" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1"/>
@@ -1023,29 +813,29 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="1"/>
@@ -1063,29 +853,29 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="1"/>
@@ -1103,29 +893,29 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="1"/>
@@ -1143,29 +933,29 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="1"/>
@@ -1183,29 +973,29 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="1"/>
@@ -1223,29 +1013,29 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="1"/>
@@ -1263,29 +1053,29 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="1"/>
@@ -1303,29 +1093,29 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="1"/>
@@ -1343,29 +1133,29 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I11" s="1"/>
@@ -1383,29 +1173,29 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="1"/>
@@ -1423,29 +1213,29 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="1"/>
@@ -1463,29 +1253,29 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="1"/>
@@ -1503,29 +1293,29 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I15" s="1"/>
@@ -1543,29 +1333,29 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="1"/>
@@ -1583,29 +1373,29 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="1" t="s">
         <v>75</v>
       </c>
       <c r="I17" s="1"/>
@@ -1623,29 +1413,29 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="I18" s="1"/>
@@ -1663,29 +1453,29 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="1" t="s">
         <v>76</v>
       </c>
       <c r="I19" s="1"/>
@@ -1703,29 +1493,29 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I20" s="1"/>
@@ -1743,29 +1533,29 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I21" s="1"/>
@@ -1783,29 +1573,29 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="I22" s="1"/>
@@ -1823,29 +1613,29 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I23" s="1"/>
@@ -1863,29 +1653,29 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="1" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="1"/>
@@ -1903,29 +1693,29 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I25" s="1"/>
@@ -1943,29 +1733,29 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="1" t="s">
         <v>91</v>
       </c>
       <c r="I26" s="1"/>
@@ -1983,29 +1773,29 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="1" t="s">
         <v>56</v>
       </c>
       <c r="I27" s="1"/>
@@ -2023,29 +1813,29 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="I28" s="1"/>
@@ -2063,29 +1853,29 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="1" t="s">
         <v>80</v>
       </c>
       <c r="I29" s="1"/>
@@ -2103,29 +1893,29 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="I30" s="1"/>
@@ -2143,29 +1933,29 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
     </row>
-    <row r="31" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I31" s="1"/>
@@ -2183,29 +1973,29 @@
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
     </row>
-    <row r="32" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="1" t="s">
         <v>62</v>
       </c>
       <c r="I32" s="1"/>
@@ -2223,29 +2013,29 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="1" t="s">
         <v>81</v>
       </c>
       <c r="I33" s="1"/>
@@ -2263,29 +2053,29 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="I34" s="1"/>
@@ -2303,29 +2093,29 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
     </row>
-    <row r="35" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="I35" s="1"/>
@@ -2343,29 +2133,29 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="H36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="I36" s="1"/>
@@ -2383,29 +2173,29 @@
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
     </row>
-    <row r="37" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="1" t="s">
         <v>88</v>
       </c>
       <c r="I37" s="1"/>
@@ -2423,29 +2213,29 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
     </row>
-    <row r="38" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H38" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I38" s="1"/>
@@ -2463,29 +2253,29 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="1" t="s">
         <v>83</v>
       </c>
       <c r="I39" s="1"/>
@@ -2503,29 +2293,29 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="H40" s="1" t="s">
         <v>85</v>
       </c>
       <c r="I40" s="1"/>
@@ -2543,31 +2333,29 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
     </row>
-    <row r="41" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="str">
-        <f>CONCATENATE("twm_", B41)</f>
-        <v>twm_Fornecedor</v>
-      </c>
-      <c r="B41" s="25" t="s">
+    <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="13" t="str">
-        <f t="shared" ref="G41:G49" si="0">CONCATENATE("twm_", H41)</f>
-        <v>twm_Fornecedor</v>
-      </c>
-      <c r="H41" s="22" t="s">
+      <c r="G41" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>93</v>
       </c>
       <c r="I41" s="1"/>
@@ -2585,33 +2373,29 @@
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
     </row>
-    <row r="42" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="str">
-        <f t="shared" ref="A42:A52" si="1">CONCATENATE("twm_", B42)</f>
-        <v>twm_Identificador</v>
-      </c>
-      <c r="B42" s="25" t="s">
+    <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="13" t="str">
-        <f>CONCATENATE("twm_", D42)</f>
-        <v>twm_Identificador</v>
-      </c>
-      <c r="D42" s="15" t="s">
+      <c r="C42" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="13" t="str">
-        <f t="shared" ref="E42:E50" si="2">CONCATENATE("twm_", F42)</f>
-        <v>twm_Identificador</v>
-      </c>
-      <c r="F42" s="17" t="s">
+      <c r="E42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Identificador</v>
-      </c>
-      <c r="H42" s="22" t="s">
+      <c r="G42" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>94</v>
       </c>
       <c r="I42" s="1"/>
@@ -2629,33 +2413,29 @@
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Categoria</v>
-      </c>
-      <c r="B43" s="25" t="s">
+    <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="13" t="str">
-        <f>CONCATENATE("twm_", D43)</f>
-        <v>twm_Categoria</v>
-      </c>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Categoria</v>
-      </c>
-      <c r="F43" s="17" t="s">
+      <c r="E43" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G43" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Categoria</v>
-      </c>
-      <c r="H43" s="22" t="s">
+      <c r="G43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>95</v>
       </c>
       <c r="I43" s="1"/>
@@ -2673,33 +2453,29 @@
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
     </row>
-    <row r="44" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Subcategoria</v>
-      </c>
-      <c r="B44" s="25" t="s">
+    <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="13" t="str">
-        <f t="shared" ref="C44:C49" si="3">CONCATENATE("twm_", D44)</f>
-        <v>twm_Data de emissão</v>
-      </c>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E44" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Subcategoria</v>
-      </c>
-      <c r="F44" s="17" t="s">
+      <c r="E44" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G44" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Subcategoria</v>
-      </c>
-      <c r="H44" s="22" t="s">
+      <c r="G44" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H44" s="3" t="s">
         <v>96</v>
       </c>
       <c r="I44" s="1"/>
@@ -2717,33 +2493,29 @@
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
     </row>
-    <row r="45" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Data de emissão</v>
-      </c>
-      <c r="B45" s="25" t="s">
+    <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v>twm_Localidade</v>
-      </c>
-      <c r="D45" s="15" t="s">
+      <c r="C45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Data de emissão</v>
-      </c>
-      <c r="F45" s="17" t="s">
+      <c r="E45" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G45" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Localidade</v>
-      </c>
-      <c r="H45" s="22" t="s">
+      <c r="G45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>100</v>
       </c>
       <c r="I45" s="1"/>
@@ -2761,33 +2533,29 @@
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
     </row>
-    <row r="46" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Status</v>
-      </c>
-      <c r="B46" s="25" t="s">
+    <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v>twm_Status</v>
-      </c>
-      <c r="D46" s="15" t="s">
+      <c r="C46" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Localidade</v>
-      </c>
-      <c r="F46" s="17" t="s">
+      <c r="E46" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G46" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Metro Quadrado</v>
-      </c>
-      <c r="H46" s="22" t="s">
+      <c r="G46" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>108</v>
       </c>
       <c r="I46" s="1"/>
@@ -2805,33 +2573,29 @@
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
     </row>
-    <row r="47" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Nota fiscal</v>
-      </c>
-      <c r="B47" s="25" t="s">
+    <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v>twm_Cód. Filial</v>
-      </c>
-      <c r="D47" s="15" t="s">
+      <c r="C47" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Status</v>
-      </c>
-      <c r="F47" s="17" t="s">
+      <c r="E47" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G47" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Alunos</v>
-      </c>
-      <c r="H47" s="22" t="s">
+      <c r="G47" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>109</v>
       </c>
       <c r="I47" s="1"/>
@@ -2849,33 +2613,29 @@
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
     </row>
-    <row r="48" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Localidade</v>
-      </c>
-      <c r="B48" s="25" t="s">
+    <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v>twm_Mês</v>
-      </c>
-      <c r="D48" s="15" t="s">
+      <c r="C48" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Cód. Filial</v>
-      </c>
-      <c r="F48" s="17" t="s">
+      <c r="E48" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G48" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_Data de emissão</v>
-      </c>
-      <c r="H48" s="22" t="s">
+      <c r="G48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>97</v>
       </c>
       <c r="I48" s="1"/>
@@ -2893,33 +2653,29 @@
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
     </row>
-    <row r="49" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Sigla</v>
-      </c>
-      <c r="B49" s="25" t="s">
+    <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v>twm_Subcategoria</v>
-      </c>
-      <c r="D49" s="16" t="s">
+      <c r="C49" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_AVB</v>
-      </c>
-      <c r="F49" s="17" t="s">
+      <c r="E49" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G49" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>twm_GRUPO</v>
-      </c>
-      <c r="H49" s="22" t="s">
+      <c r="G49" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>110</v>
       </c>
       <c r="I49" s="1"/>
@@ -2937,23 +2693,23 @@
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
     </row>
-    <row r="50" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Regional</v>
-      </c>
-      <c r="B50" s="25" t="s">
+    <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>twm_Nota fiscal</v>
-      </c>
-      <c r="F50" s="17" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -2969,16 +2725,19 @@
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
     </row>
-    <row r="51" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_Divisional</v>
-      </c>
-      <c r="B51" s="25" t="s">
+    <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -2994,14 +2753,14 @@
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
     </row>
-    <row r="52" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>twm_ES</v>
-      </c>
-      <c r="B52" s="25" t="s">
+    <row r="52" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="C52" s="3"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -20702,8 +20461,6 @@
     <row r="937" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A937" s="1"/>
       <c r="B937" s="1"/>
-      <c r="G937" s="1"/>
-      <c r="H937" s="1"/>
       <c r="I937" s="1"/>
       <c r="J937" s="1"/>
       <c r="K937" s="1"/>
@@ -20719,1124 +20476,6 @@
       <c r="U937" s="1"/>
       <c r="V937" s="1"/>
     </row>
-    <row r="938" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A938" s="1"/>
-      <c r="B938" s="1"/>
-      <c r="G938" s="1"/>
-      <c r="H938" s="1"/>
-      <c r="I938" s="1"/>
-      <c r="J938" s="1"/>
-      <c r="K938" s="1"/>
-      <c r="L938" s="1"/>
-      <c r="M938" s="1"/>
-      <c r="N938" s="1"/>
-      <c r="O938" s="1"/>
-      <c r="P938" s="1"/>
-      <c r="Q938" s="1"/>
-      <c r="R938" s="1"/>
-      <c r="S938" s="1"/>
-      <c r="T938" s="1"/>
-      <c r="U938" s="1"/>
-      <c r="V938" s="1"/>
-    </row>
-    <row r="939" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A939" s="1"/>
-      <c r="B939" s="1"/>
-      <c r="G939" s="1"/>
-      <c r="H939" s="1"/>
-      <c r="I939" s="1"/>
-      <c r="J939" s="1"/>
-      <c r="K939" s="1"/>
-      <c r="L939" s="1"/>
-      <c r="M939" s="1"/>
-      <c r="N939" s="1"/>
-      <c r="O939" s="1"/>
-      <c r="P939" s="1"/>
-      <c r="Q939" s="1"/>
-      <c r="R939" s="1"/>
-      <c r="S939" s="1"/>
-      <c r="T939" s="1"/>
-      <c r="U939" s="1"/>
-      <c r="V939" s="1"/>
-    </row>
-    <row r="940" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A940" s="1"/>
-      <c r="B940" s="1"/>
-      <c r="G940" s="1"/>
-      <c r="H940" s="1"/>
-      <c r="I940" s="1"/>
-      <c r="J940" s="1"/>
-      <c r="K940" s="1"/>
-      <c r="L940" s="1"/>
-      <c r="M940" s="1"/>
-      <c r="N940" s="1"/>
-      <c r="O940" s="1"/>
-      <c r="P940" s="1"/>
-      <c r="Q940" s="1"/>
-      <c r="R940" s="1"/>
-      <c r="S940" s="1"/>
-      <c r="T940" s="1"/>
-      <c r="U940" s="1"/>
-      <c r="V940" s="1"/>
-    </row>
-    <row r="941" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A941" s="1"/>
-      <c r="B941" s="1"/>
-      <c r="G941" s="1"/>
-      <c r="H941" s="1"/>
-      <c r="I941" s="1"/>
-      <c r="J941" s="1"/>
-      <c r="K941" s="1"/>
-      <c r="L941" s="1"/>
-      <c r="M941" s="1"/>
-      <c r="N941" s="1"/>
-      <c r="O941" s="1"/>
-      <c r="P941" s="1"/>
-      <c r="Q941" s="1"/>
-      <c r="R941" s="1"/>
-      <c r="S941" s="1"/>
-      <c r="T941" s="1"/>
-      <c r="U941" s="1"/>
-      <c r="V941" s="1"/>
-    </row>
-    <row r="942" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A942" s="1"/>
-      <c r="B942" s="1"/>
-      <c r="G942" s="1"/>
-      <c r="H942" s="1"/>
-      <c r="I942" s="1"/>
-      <c r="J942" s="1"/>
-      <c r="K942" s="1"/>
-      <c r="L942" s="1"/>
-      <c r="M942" s="1"/>
-      <c r="N942" s="1"/>
-      <c r="O942" s="1"/>
-      <c r="P942" s="1"/>
-      <c r="Q942" s="1"/>
-      <c r="R942" s="1"/>
-      <c r="S942" s="1"/>
-      <c r="T942" s="1"/>
-      <c r="U942" s="1"/>
-      <c r="V942" s="1"/>
-    </row>
-    <row r="943" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A943" s="1"/>
-      <c r="B943" s="1"/>
-      <c r="G943" s="1"/>
-      <c r="H943" s="1"/>
-      <c r="I943" s="1"/>
-      <c r="J943" s="1"/>
-      <c r="K943" s="1"/>
-      <c r="L943" s="1"/>
-      <c r="M943" s="1"/>
-      <c r="N943" s="1"/>
-      <c r="O943" s="1"/>
-      <c r="P943" s="1"/>
-      <c r="Q943" s="1"/>
-      <c r="R943" s="1"/>
-      <c r="S943" s="1"/>
-      <c r="T943" s="1"/>
-      <c r="U943" s="1"/>
-      <c r="V943" s="1"/>
-    </row>
-    <row r="944" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A944" s="1"/>
-      <c r="B944" s="1"/>
-      <c r="G944" s="1"/>
-      <c r="H944" s="1"/>
-      <c r="I944" s="1"/>
-      <c r="J944" s="1"/>
-      <c r="K944" s="1"/>
-      <c r="L944" s="1"/>
-      <c r="M944" s="1"/>
-      <c r="N944" s="1"/>
-      <c r="O944" s="1"/>
-      <c r="P944" s="1"/>
-      <c r="Q944" s="1"/>
-      <c r="R944" s="1"/>
-      <c r="S944" s="1"/>
-      <c r="T944" s="1"/>
-      <c r="U944" s="1"/>
-      <c r="V944" s="1"/>
-    </row>
-    <row r="945" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A945" s="1"/>
-      <c r="B945" s="1"/>
-      <c r="G945" s="1"/>
-      <c r="H945" s="1"/>
-      <c r="I945" s="1"/>
-      <c r="J945" s="1"/>
-      <c r="K945" s="1"/>
-      <c r="L945" s="1"/>
-      <c r="M945" s="1"/>
-      <c r="N945" s="1"/>
-      <c r="O945" s="1"/>
-      <c r="P945" s="1"/>
-      <c r="Q945" s="1"/>
-      <c r="R945" s="1"/>
-      <c r="S945" s="1"/>
-      <c r="T945" s="1"/>
-      <c r="U945" s="1"/>
-      <c r="V945" s="1"/>
-    </row>
-    <row r="946" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A946" s="1"/>
-      <c r="B946" s="1"/>
-      <c r="G946" s="1"/>
-      <c r="H946" s="1"/>
-      <c r="I946" s="1"/>
-      <c r="J946" s="1"/>
-      <c r="K946" s="1"/>
-      <c r="L946" s="1"/>
-      <c r="M946" s="1"/>
-      <c r="N946" s="1"/>
-      <c r="O946" s="1"/>
-      <c r="P946" s="1"/>
-      <c r="Q946" s="1"/>
-      <c r="R946" s="1"/>
-      <c r="S946" s="1"/>
-      <c r="T946" s="1"/>
-      <c r="U946" s="1"/>
-      <c r="V946" s="1"/>
-    </row>
-    <row r="947" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A947" s="1"/>
-      <c r="B947" s="1"/>
-      <c r="G947" s="1"/>
-      <c r="H947" s="1"/>
-      <c r="I947" s="1"/>
-      <c r="J947" s="1"/>
-      <c r="K947" s="1"/>
-      <c r="L947" s="1"/>
-      <c r="M947" s="1"/>
-      <c r="N947" s="1"/>
-      <c r="O947" s="1"/>
-      <c r="P947" s="1"/>
-      <c r="Q947" s="1"/>
-      <c r="R947" s="1"/>
-      <c r="S947" s="1"/>
-      <c r="T947" s="1"/>
-      <c r="U947" s="1"/>
-      <c r="V947" s="1"/>
-    </row>
-    <row r="948" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A948" s="1"/>
-      <c r="B948" s="1"/>
-      <c r="G948" s="1"/>
-      <c r="H948" s="1"/>
-      <c r="I948" s="1"/>
-      <c r="J948" s="1"/>
-      <c r="K948" s="1"/>
-      <c r="L948" s="1"/>
-      <c r="M948" s="1"/>
-      <c r="N948" s="1"/>
-      <c r="O948" s="1"/>
-      <c r="P948" s="1"/>
-      <c r="Q948" s="1"/>
-      <c r="R948" s="1"/>
-      <c r="S948" s="1"/>
-      <c r="T948" s="1"/>
-      <c r="U948" s="1"/>
-      <c r="V948" s="1"/>
-    </row>
-    <row r="949" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A949" s="1"/>
-      <c r="B949" s="1"/>
-      <c r="G949" s="1"/>
-      <c r="H949" s="1"/>
-      <c r="I949" s="1"/>
-      <c r="J949" s="1"/>
-      <c r="K949" s="1"/>
-      <c r="L949" s="1"/>
-      <c r="M949" s="1"/>
-      <c r="N949" s="1"/>
-      <c r="O949" s="1"/>
-      <c r="P949" s="1"/>
-      <c r="Q949" s="1"/>
-      <c r="R949" s="1"/>
-      <c r="S949" s="1"/>
-      <c r="T949" s="1"/>
-      <c r="U949" s="1"/>
-      <c r="V949" s="1"/>
-    </row>
-    <row r="950" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A950" s="1"/>
-      <c r="B950" s="1"/>
-      <c r="G950" s="1"/>
-      <c r="H950" s="1"/>
-      <c r="I950" s="1"/>
-      <c r="J950" s="1"/>
-      <c r="K950" s="1"/>
-      <c r="L950" s="1"/>
-      <c r="M950" s="1"/>
-      <c r="N950" s="1"/>
-      <c r="O950" s="1"/>
-      <c r="P950" s="1"/>
-      <c r="Q950" s="1"/>
-      <c r="R950" s="1"/>
-      <c r="S950" s="1"/>
-      <c r="T950" s="1"/>
-      <c r="U950" s="1"/>
-      <c r="V950" s="1"/>
-    </row>
-    <row r="951" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A951" s="1"/>
-      <c r="B951" s="1"/>
-      <c r="G951" s="1"/>
-      <c r="H951" s="1"/>
-      <c r="I951" s="1"/>
-      <c r="J951" s="1"/>
-      <c r="K951" s="1"/>
-      <c r="L951" s="1"/>
-      <c r="M951" s="1"/>
-      <c r="N951" s="1"/>
-      <c r="O951" s="1"/>
-      <c r="P951" s="1"/>
-      <c r="Q951" s="1"/>
-      <c r="R951" s="1"/>
-      <c r="S951" s="1"/>
-      <c r="T951" s="1"/>
-      <c r="U951" s="1"/>
-      <c r="V951" s="1"/>
-    </row>
-    <row r="952" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A952" s="1"/>
-      <c r="B952" s="1"/>
-      <c r="G952" s="1"/>
-      <c r="H952" s="1"/>
-      <c r="I952" s="1"/>
-      <c r="J952" s="1"/>
-      <c r="K952" s="1"/>
-      <c r="L952" s="1"/>
-      <c r="M952" s="1"/>
-      <c r="N952" s="1"/>
-      <c r="O952" s="1"/>
-      <c r="P952" s="1"/>
-      <c r="Q952" s="1"/>
-      <c r="R952" s="1"/>
-      <c r="S952" s="1"/>
-      <c r="T952" s="1"/>
-      <c r="U952" s="1"/>
-      <c r="V952" s="1"/>
-    </row>
-    <row r="953" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A953" s="1"/>
-      <c r="B953" s="1"/>
-      <c r="G953" s="1"/>
-      <c r="H953" s="1"/>
-      <c r="I953" s="1"/>
-      <c r="J953" s="1"/>
-      <c r="K953" s="1"/>
-      <c r="L953" s="1"/>
-      <c r="M953" s="1"/>
-      <c r="N953" s="1"/>
-      <c r="O953" s="1"/>
-      <c r="P953" s="1"/>
-      <c r="Q953" s="1"/>
-      <c r="R953" s="1"/>
-      <c r="S953" s="1"/>
-      <c r="T953" s="1"/>
-      <c r="U953" s="1"/>
-      <c r="V953" s="1"/>
-    </row>
-    <row r="954" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A954" s="1"/>
-      <c r="B954" s="1"/>
-      <c r="G954" s="1"/>
-      <c r="H954" s="1"/>
-      <c r="I954" s="1"/>
-      <c r="J954" s="1"/>
-      <c r="K954" s="1"/>
-      <c r="L954" s="1"/>
-      <c r="M954" s="1"/>
-      <c r="N954" s="1"/>
-      <c r="O954" s="1"/>
-      <c r="P954" s="1"/>
-      <c r="Q954" s="1"/>
-      <c r="R954" s="1"/>
-      <c r="S954" s="1"/>
-      <c r="T954" s="1"/>
-      <c r="U954" s="1"/>
-      <c r="V954" s="1"/>
-    </row>
-    <row r="955" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A955" s="1"/>
-      <c r="B955" s="1"/>
-      <c r="G955" s="1"/>
-      <c r="H955" s="1"/>
-      <c r="I955" s="1"/>
-      <c r="J955" s="1"/>
-      <c r="K955" s="1"/>
-      <c r="L955" s="1"/>
-      <c r="M955" s="1"/>
-      <c r="N955" s="1"/>
-      <c r="O955" s="1"/>
-      <c r="P955" s="1"/>
-      <c r="Q955" s="1"/>
-      <c r="R955" s="1"/>
-      <c r="S955" s="1"/>
-      <c r="T955" s="1"/>
-      <c r="U955" s="1"/>
-      <c r="V955" s="1"/>
-    </row>
-    <row r="956" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A956" s="1"/>
-      <c r="B956" s="1"/>
-      <c r="G956" s="1"/>
-      <c r="H956" s="1"/>
-      <c r="I956" s="1"/>
-      <c r="J956" s="1"/>
-      <c r="K956" s="1"/>
-      <c r="L956" s="1"/>
-      <c r="M956" s="1"/>
-      <c r="N956" s="1"/>
-      <c r="O956" s="1"/>
-      <c r="P956" s="1"/>
-      <c r="Q956" s="1"/>
-      <c r="R956" s="1"/>
-      <c r="S956" s="1"/>
-      <c r="T956" s="1"/>
-      <c r="U956" s="1"/>
-      <c r="V956" s="1"/>
-    </row>
-    <row r="957" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A957" s="1"/>
-      <c r="B957" s="1"/>
-      <c r="G957" s="1"/>
-      <c r="H957" s="1"/>
-      <c r="I957" s="1"/>
-      <c r="J957" s="1"/>
-      <c r="K957" s="1"/>
-      <c r="L957" s="1"/>
-      <c r="M957" s="1"/>
-      <c r="N957" s="1"/>
-      <c r="O957" s="1"/>
-      <c r="P957" s="1"/>
-      <c r="Q957" s="1"/>
-      <c r="R957" s="1"/>
-      <c r="S957" s="1"/>
-      <c r="T957" s="1"/>
-      <c r="U957" s="1"/>
-      <c r="V957" s="1"/>
-    </row>
-    <row r="958" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A958" s="1"/>
-      <c r="B958" s="1"/>
-      <c r="G958" s="1"/>
-      <c r="H958" s="1"/>
-      <c r="I958" s="1"/>
-      <c r="J958" s="1"/>
-      <c r="K958" s="1"/>
-      <c r="L958" s="1"/>
-      <c r="M958" s="1"/>
-      <c r="N958" s="1"/>
-      <c r="O958" s="1"/>
-      <c r="P958" s="1"/>
-      <c r="Q958" s="1"/>
-      <c r="R958" s="1"/>
-      <c r="S958" s="1"/>
-      <c r="T958" s="1"/>
-      <c r="U958" s="1"/>
-      <c r="V958" s="1"/>
-    </row>
-    <row r="959" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A959" s="1"/>
-      <c r="B959" s="1"/>
-      <c r="G959" s="1"/>
-      <c r="H959" s="1"/>
-      <c r="I959" s="1"/>
-      <c r="J959" s="1"/>
-      <c r="K959" s="1"/>
-      <c r="L959" s="1"/>
-      <c r="M959" s="1"/>
-      <c r="N959" s="1"/>
-      <c r="O959" s="1"/>
-      <c r="P959" s="1"/>
-      <c r="Q959" s="1"/>
-      <c r="R959" s="1"/>
-      <c r="S959" s="1"/>
-      <c r="T959" s="1"/>
-      <c r="U959" s="1"/>
-      <c r="V959" s="1"/>
-    </row>
-    <row r="960" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A960" s="1"/>
-      <c r="B960" s="1"/>
-      <c r="G960" s="1"/>
-      <c r="H960" s="1"/>
-      <c r="I960" s="1"/>
-      <c r="J960" s="1"/>
-      <c r="K960" s="1"/>
-      <c r="L960" s="1"/>
-      <c r="M960" s="1"/>
-      <c r="N960" s="1"/>
-      <c r="O960" s="1"/>
-      <c r="P960" s="1"/>
-      <c r="Q960" s="1"/>
-      <c r="R960" s="1"/>
-      <c r="S960" s="1"/>
-      <c r="T960" s="1"/>
-      <c r="U960" s="1"/>
-      <c r="V960" s="1"/>
-    </row>
-    <row r="961" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A961" s="1"/>
-      <c r="B961" s="1"/>
-      <c r="G961" s="1"/>
-      <c r="H961" s="1"/>
-      <c r="I961" s="1"/>
-      <c r="J961" s="1"/>
-      <c r="K961" s="1"/>
-      <c r="L961" s="1"/>
-      <c r="M961" s="1"/>
-      <c r="N961" s="1"/>
-      <c r="O961" s="1"/>
-      <c r="P961" s="1"/>
-      <c r="Q961" s="1"/>
-      <c r="R961" s="1"/>
-      <c r="S961" s="1"/>
-      <c r="T961" s="1"/>
-      <c r="U961" s="1"/>
-      <c r="V961" s="1"/>
-    </row>
-    <row r="962" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A962" s="1"/>
-      <c r="B962" s="1"/>
-      <c r="G962" s="1"/>
-      <c r="H962" s="1"/>
-      <c r="I962" s="1"/>
-      <c r="J962" s="1"/>
-      <c r="K962" s="1"/>
-      <c r="L962" s="1"/>
-      <c r="M962" s="1"/>
-      <c r="N962" s="1"/>
-      <c r="O962" s="1"/>
-      <c r="P962" s="1"/>
-      <c r="Q962" s="1"/>
-      <c r="R962" s="1"/>
-      <c r="S962" s="1"/>
-      <c r="T962" s="1"/>
-      <c r="U962" s="1"/>
-      <c r="V962" s="1"/>
-    </row>
-    <row r="963" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A963" s="1"/>
-      <c r="B963" s="1"/>
-      <c r="G963" s="1"/>
-      <c r="H963" s="1"/>
-      <c r="I963" s="1"/>
-      <c r="J963" s="1"/>
-      <c r="K963" s="1"/>
-      <c r="L963" s="1"/>
-      <c r="M963" s="1"/>
-      <c r="N963" s="1"/>
-      <c r="O963" s="1"/>
-      <c r="P963" s="1"/>
-      <c r="Q963" s="1"/>
-      <c r="R963" s="1"/>
-      <c r="S963" s="1"/>
-      <c r="T963" s="1"/>
-      <c r="U963" s="1"/>
-      <c r="V963" s="1"/>
-    </row>
-    <row r="964" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A964" s="1"/>
-      <c r="B964" s="1"/>
-      <c r="G964" s="1"/>
-      <c r="H964" s="1"/>
-      <c r="I964" s="1"/>
-      <c r="J964" s="1"/>
-      <c r="K964" s="1"/>
-      <c r="L964" s="1"/>
-      <c r="M964" s="1"/>
-      <c r="N964" s="1"/>
-      <c r="O964" s="1"/>
-      <c r="P964" s="1"/>
-      <c r="Q964" s="1"/>
-      <c r="R964" s="1"/>
-      <c r="S964" s="1"/>
-      <c r="T964" s="1"/>
-      <c r="U964" s="1"/>
-      <c r="V964" s="1"/>
-    </row>
-    <row r="965" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A965" s="1"/>
-      <c r="B965" s="1"/>
-      <c r="G965" s="1"/>
-      <c r="H965" s="1"/>
-      <c r="I965" s="1"/>
-      <c r="J965" s="1"/>
-      <c r="K965" s="1"/>
-      <c r="L965" s="1"/>
-      <c r="M965" s="1"/>
-      <c r="N965" s="1"/>
-      <c r="O965" s="1"/>
-      <c r="P965" s="1"/>
-      <c r="Q965" s="1"/>
-      <c r="R965" s="1"/>
-      <c r="S965" s="1"/>
-      <c r="T965" s="1"/>
-      <c r="U965" s="1"/>
-      <c r="V965" s="1"/>
-    </row>
-    <row r="966" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A966" s="1"/>
-      <c r="B966" s="1"/>
-      <c r="G966" s="1"/>
-      <c r="H966" s="1"/>
-      <c r="I966" s="1"/>
-      <c r="J966" s="1"/>
-      <c r="K966" s="1"/>
-      <c r="L966" s="1"/>
-      <c r="M966" s="1"/>
-      <c r="N966" s="1"/>
-      <c r="O966" s="1"/>
-      <c r="P966" s="1"/>
-      <c r="Q966" s="1"/>
-      <c r="R966" s="1"/>
-      <c r="S966" s="1"/>
-      <c r="T966" s="1"/>
-      <c r="U966" s="1"/>
-      <c r="V966" s="1"/>
-    </row>
-    <row r="967" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A967" s="1"/>
-      <c r="B967" s="1"/>
-      <c r="G967" s="1"/>
-      <c r="H967" s="1"/>
-      <c r="I967" s="1"/>
-      <c r="J967" s="1"/>
-      <c r="K967" s="1"/>
-      <c r="L967" s="1"/>
-      <c r="M967" s="1"/>
-      <c r="N967" s="1"/>
-      <c r="O967" s="1"/>
-      <c r="P967" s="1"/>
-      <c r="Q967" s="1"/>
-      <c r="R967" s="1"/>
-      <c r="S967" s="1"/>
-      <c r="T967" s="1"/>
-      <c r="U967" s="1"/>
-      <c r="V967" s="1"/>
-    </row>
-    <row r="968" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A968" s="1"/>
-      <c r="B968" s="1"/>
-      <c r="G968" s="1"/>
-      <c r="H968" s="1"/>
-      <c r="I968" s="1"/>
-      <c r="J968" s="1"/>
-      <c r="K968" s="1"/>
-      <c r="L968" s="1"/>
-      <c r="M968" s="1"/>
-      <c r="N968" s="1"/>
-      <c r="O968" s="1"/>
-      <c r="P968" s="1"/>
-      <c r="Q968" s="1"/>
-      <c r="R968" s="1"/>
-      <c r="S968" s="1"/>
-      <c r="T968" s="1"/>
-      <c r="U968" s="1"/>
-      <c r="V968" s="1"/>
-    </row>
-    <row r="969" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A969" s="1"/>
-      <c r="B969" s="1"/>
-      <c r="G969" s="1"/>
-      <c r="H969" s="1"/>
-      <c r="I969" s="1"/>
-      <c r="J969" s="1"/>
-      <c r="K969" s="1"/>
-      <c r="L969" s="1"/>
-      <c r="M969" s="1"/>
-      <c r="N969" s="1"/>
-      <c r="O969" s="1"/>
-      <c r="P969" s="1"/>
-      <c r="Q969" s="1"/>
-      <c r="R969" s="1"/>
-      <c r="S969" s="1"/>
-      <c r="T969" s="1"/>
-      <c r="U969" s="1"/>
-      <c r="V969" s="1"/>
-    </row>
-    <row r="970" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A970" s="1"/>
-      <c r="B970" s="1"/>
-      <c r="G970" s="1"/>
-      <c r="H970" s="1"/>
-      <c r="I970" s="1"/>
-      <c r="J970" s="1"/>
-      <c r="K970" s="1"/>
-      <c r="L970" s="1"/>
-      <c r="M970" s="1"/>
-      <c r="N970" s="1"/>
-      <c r="O970" s="1"/>
-      <c r="P970" s="1"/>
-      <c r="Q970" s="1"/>
-      <c r="R970" s="1"/>
-      <c r="S970" s="1"/>
-      <c r="T970" s="1"/>
-      <c r="U970" s="1"/>
-      <c r="V970" s="1"/>
-    </row>
-    <row r="971" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A971" s="1"/>
-      <c r="B971" s="1"/>
-      <c r="G971" s="1"/>
-      <c r="H971" s="1"/>
-      <c r="I971" s="1"/>
-      <c r="J971" s="1"/>
-      <c r="K971" s="1"/>
-      <c r="L971" s="1"/>
-      <c r="M971" s="1"/>
-      <c r="N971" s="1"/>
-      <c r="O971" s="1"/>
-      <c r="P971" s="1"/>
-      <c r="Q971" s="1"/>
-      <c r="R971" s="1"/>
-      <c r="S971" s="1"/>
-      <c r="T971" s="1"/>
-      <c r="U971" s="1"/>
-      <c r="V971" s="1"/>
-    </row>
-    <row r="972" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A972" s="1"/>
-      <c r="B972" s="1"/>
-      <c r="G972" s="1"/>
-      <c r="H972" s="1"/>
-      <c r="I972" s="1"/>
-      <c r="J972" s="1"/>
-      <c r="K972" s="1"/>
-      <c r="L972" s="1"/>
-      <c r="M972" s="1"/>
-      <c r="N972" s="1"/>
-      <c r="O972" s="1"/>
-      <c r="P972" s="1"/>
-      <c r="Q972" s="1"/>
-      <c r="R972" s="1"/>
-      <c r="S972" s="1"/>
-      <c r="T972" s="1"/>
-      <c r="U972" s="1"/>
-      <c r="V972" s="1"/>
-    </row>
-    <row r="973" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A973" s="1"/>
-      <c r="B973" s="1"/>
-      <c r="G973" s="1"/>
-      <c r="H973" s="1"/>
-      <c r="I973" s="1"/>
-      <c r="J973" s="1"/>
-      <c r="K973" s="1"/>
-      <c r="L973" s="1"/>
-      <c r="M973" s="1"/>
-      <c r="N973" s="1"/>
-      <c r="O973" s="1"/>
-      <c r="P973" s="1"/>
-      <c r="Q973" s="1"/>
-      <c r="R973" s="1"/>
-      <c r="S973" s="1"/>
-      <c r="T973" s="1"/>
-      <c r="U973" s="1"/>
-      <c r="V973" s="1"/>
-    </row>
-    <row r="974" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A974" s="1"/>
-      <c r="B974" s="1"/>
-      <c r="G974" s="1"/>
-      <c r="H974" s="1"/>
-      <c r="I974" s="1"/>
-      <c r="J974" s="1"/>
-      <c r="K974" s="1"/>
-      <c r="L974" s="1"/>
-      <c r="M974" s="1"/>
-      <c r="N974" s="1"/>
-      <c r="O974" s="1"/>
-      <c r="P974" s="1"/>
-      <c r="Q974" s="1"/>
-      <c r="R974" s="1"/>
-      <c r="S974" s="1"/>
-      <c r="T974" s="1"/>
-      <c r="U974" s="1"/>
-      <c r="V974" s="1"/>
-    </row>
-    <row r="975" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A975" s="1"/>
-      <c r="B975" s="1"/>
-      <c r="G975" s="1"/>
-      <c r="H975" s="1"/>
-      <c r="I975" s="1"/>
-      <c r="J975" s="1"/>
-      <c r="K975" s="1"/>
-      <c r="L975" s="1"/>
-      <c r="M975" s="1"/>
-      <c r="N975" s="1"/>
-      <c r="O975" s="1"/>
-      <c r="P975" s="1"/>
-      <c r="Q975" s="1"/>
-      <c r="R975" s="1"/>
-      <c r="S975" s="1"/>
-      <c r="T975" s="1"/>
-      <c r="U975" s="1"/>
-      <c r="V975" s="1"/>
-    </row>
-    <row r="976" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A976" s="1"/>
-      <c r="B976" s="1"/>
-      <c r="G976" s="1"/>
-      <c r="H976" s="1"/>
-      <c r="I976" s="1"/>
-      <c r="J976" s="1"/>
-      <c r="K976" s="1"/>
-      <c r="L976" s="1"/>
-      <c r="M976" s="1"/>
-      <c r="N976" s="1"/>
-      <c r="O976" s="1"/>
-      <c r="P976" s="1"/>
-      <c r="Q976" s="1"/>
-      <c r="R976" s="1"/>
-      <c r="S976" s="1"/>
-      <c r="T976" s="1"/>
-      <c r="U976" s="1"/>
-      <c r="V976" s="1"/>
-    </row>
-    <row r="977" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A977" s="1"/>
-      <c r="B977" s="1"/>
-      <c r="G977" s="1"/>
-      <c r="H977" s="1"/>
-      <c r="I977" s="1"/>
-      <c r="J977" s="1"/>
-      <c r="K977" s="1"/>
-      <c r="L977" s="1"/>
-      <c r="M977" s="1"/>
-      <c r="N977" s="1"/>
-      <c r="O977" s="1"/>
-      <c r="P977" s="1"/>
-      <c r="Q977" s="1"/>
-      <c r="R977" s="1"/>
-      <c r="S977" s="1"/>
-      <c r="T977" s="1"/>
-      <c r="U977" s="1"/>
-      <c r="V977" s="1"/>
-    </row>
-    <row r="978" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A978" s="1"/>
-      <c r="B978" s="1"/>
-      <c r="G978" s="1"/>
-      <c r="H978" s="1"/>
-      <c r="I978" s="1"/>
-      <c r="J978" s="1"/>
-      <c r="K978" s="1"/>
-      <c r="L978" s="1"/>
-      <c r="M978" s="1"/>
-      <c r="N978" s="1"/>
-      <c r="O978" s="1"/>
-      <c r="P978" s="1"/>
-      <c r="Q978" s="1"/>
-      <c r="R978" s="1"/>
-      <c r="S978" s="1"/>
-      <c r="T978" s="1"/>
-      <c r="U978" s="1"/>
-      <c r="V978" s="1"/>
-    </row>
-    <row r="979" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A979" s="1"/>
-      <c r="B979" s="1"/>
-      <c r="G979" s="1"/>
-      <c r="H979" s="1"/>
-      <c r="I979" s="1"/>
-      <c r="J979" s="1"/>
-      <c r="K979" s="1"/>
-      <c r="L979" s="1"/>
-      <c r="M979" s="1"/>
-      <c r="N979" s="1"/>
-      <c r="O979" s="1"/>
-      <c r="P979" s="1"/>
-      <c r="Q979" s="1"/>
-      <c r="R979" s="1"/>
-      <c r="S979" s="1"/>
-      <c r="T979" s="1"/>
-      <c r="U979" s="1"/>
-      <c r="V979" s="1"/>
-    </row>
-    <row r="980" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A980" s="1"/>
-      <c r="B980" s="1"/>
-      <c r="G980" s="1"/>
-      <c r="H980" s="1"/>
-      <c r="I980" s="1"/>
-      <c r="J980" s="1"/>
-      <c r="K980" s="1"/>
-      <c r="L980" s="1"/>
-      <c r="M980" s="1"/>
-      <c r="N980" s="1"/>
-      <c r="O980" s="1"/>
-      <c r="P980" s="1"/>
-      <c r="Q980" s="1"/>
-      <c r="R980" s="1"/>
-      <c r="S980" s="1"/>
-      <c r="T980" s="1"/>
-      <c r="U980" s="1"/>
-      <c r="V980" s="1"/>
-    </row>
-    <row r="981" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A981" s="1"/>
-      <c r="B981" s="1"/>
-      <c r="G981" s="1"/>
-      <c r="H981" s="1"/>
-      <c r="I981" s="1"/>
-      <c r="J981" s="1"/>
-      <c r="K981" s="1"/>
-      <c r="L981" s="1"/>
-      <c r="M981" s="1"/>
-      <c r="N981" s="1"/>
-      <c r="O981" s="1"/>
-      <c r="P981" s="1"/>
-      <c r="Q981" s="1"/>
-      <c r="R981" s="1"/>
-      <c r="S981" s="1"/>
-      <c r="T981" s="1"/>
-      <c r="U981" s="1"/>
-      <c r="V981" s="1"/>
-    </row>
-    <row r="982" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A982" s="1"/>
-      <c r="B982" s="1"/>
-      <c r="G982" s="1"/>
-      <c r="H982" s="1"/>
-      <c r="I982" s="1"/>
-      <c r="J982" s="1"/>
-      <c r="K982" s="1"/>
-      <c r="L982" s="1"/>
-      <c r="M982" s="1"/>
-      <c r="N982" s="1"/>
-      <c r="O982" s="1"/>
-      <c r="P982" s="1"/>
-      <c r="Q982" s="1"/>
-      <c r="R982" s="1"/>
-      <c r="S982" s="1"/>
-      <c r="T982" s="1"/>
-      <c r="U982" s="1"/>
-      <c r="V982" s="1"/>
-    </row>
-    <row r="983" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A983" s="1"/>
-      <c r="B983" s="1"/>
-      <c r="G983" s="1"/>
-      <c r="H983" s="1"/>
-      <c r="I983" s="1"/>
-      <c r="J983" s="1"/>
-      <c r="K983" s="1"/>
-      <c r="L983" s="1"/>
-      <c r="M983" s="1"/>
-      <c r="N983" s="1"/>
-      <c r="O983" s="1"/>
-      <c r="P983" s="1"/>
-      <c r="Q983" s="1"/>
-      <c r="R983" s="1"/>
-      <c r="S983" s="1"/>
-      <c r="T983" s="1"/>
-      <c r="U983" s="1"/>
-      <c r="V983" s="1"/>
-    </row>
-    <row r="984" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A984" s="1"/>
-      <c r="B984" s="1"/>
-      <c r="G984" s="1"/>
-      <c r="H984" s="1"/>
-      <c r="I984" s="1"/>
-      <c r="J984" s="1"/>
-      <c r="K984" s="1"/>
-      <c r="L984" s="1"/>
-      <c r="M984" s="1"/>
-      <c r="N984" s="1"/>
-      <c r="O984" s="1"/>
-      <c r="P984" s="1"/>
-      <c r="Q984" s="1"/>
-      <c r="R984" s="1"/>
-      <c r="S984" s="1"/>
-      <c r="T984" s="1"/>
-      <c r="U984" s="1"/>
-      <c r="V984" s="1"/>
-    </row>
-    <row r="985" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A985" s="1"/>
-      <c r="B985" s="1"/>
-      <c r="G985" s="1"/>
-      <c r="H985" s="1"/>
-      <c r="I985" s="1"/>
-      <c r="J985" s="1"/>
-      <c r="K985" s="1"/>
-      <c r="L985" s="1"/>
-      <c r="M985" s="1"/>
-      <c r="N985" s="1"/>
-      <c r="O985" s="1"/>
-      <c r="P985" s="1"/>
-      <c r="Q985" s="1"/>
-      <c r="R985" s="1"/>
-      <c r="S985" s="1"/>
-      <c r="T985" s="1"/>
-      <c r="U985" s="1"/>
-      <c r="V985" s="1"/>
-    </row>
-    <row r="986" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A986" s="1"/>
-      <c r="B986" s="1"/>
-      <c r="G986" s="1"/>
-      <c r="H986" s="1"/>
-      <c r="I986" s="1"/>
-      <c r="J986" s="1"/>
-      <c r="K986" s="1"/>
-      <c r="L986" s="1"/>
-      <c r="M986" s="1"/>
-      <c r="N986" s="1"/>
-      <c r="O986" s="1"/>
-      <c r="P986" s="1"/>
-      <c r="Q986" s="1"/>
-      <c r="R986" s="1"/>
-      <c r="S986" s="1"/>
-      <c r="T986" s="1"/>
-      <c r="U986" s="1"/>
-      <c r="V986" s="1"/>
-    </row>
-    <row r="987" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="G987" s="1"/>
-      <c r="H987" s="1"/>
-      <c r="I987" s="1"/>
-      <c r="J987" s="1"/>
-      <c r="K987" s="1"/>
-      <c r="L987" s="1"/>
-      <c r="M987" s="1"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="1"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-      <c r="T987" s="1"/>
-      <c r="U987" s="1"/>
-      <c r="V987" s="1"/>
-    </row>
-    <row r="988" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A988" s="1"/>
-      <c r="B988" s="1"/>
-      <c r="G988" s="1"/>
-      <c r="H988" s="1"/>
-      <c r="I988" s="1"/>
-      <c r="J988" s="1"/>
-      <c r="K988" s="1"/>
-      <c r="L988" s="1"/>
-      <c r="M988" s="1"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="1"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-      <c r="T988" s="1"/>
-      <c r="U988" s="1"/>
-      <c r="V988" s="1"/>
-    </row>
-    <row r="989" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A989" s="1"/>
-      <c r="B989" s="1"/>
-      <c r="G989" s="1"/>
-      <c r="H989" s="1"/>
-      <c r="I989" s="1"/>
-      <c r="J989" s="1"/>
-      <c r="K989" s="1"/>
-      <c r="L989" s="1"/>
-      <c r="M989" s="1"/>
-      <c r="N989" s="1"/>
-      <c r="O989" s="1"/>
-      <c r="P989" s="1"/>
-      <c r="Q989" s="1"/>
-      <c r="R989" s="1"/>
-      <c r="S989" s="1"/>
-      <c r="T989" s="1"/>
-      <c r="U989" s="1"/>
-      <c r="V989" s="1"/>
-    </row>
-    <row r="990" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A990" s="1"/>
-      <c r="B990" s="1"/>
-      <c r="G990" s="1"/>
-      <c r="H990" s="1"/>
-      <c r="I990" s="1"/>
-      <c r="J990" s="1"/>
-      <c r="K990" s="1"/>
-      <c r="L990" s="1"/>
-      <c r="M990" s="1"/>
-      <c r="N990" s="1"/>
-      <c r="O990" s="1"/>
-      <c r="P990" s="1"/>
-      <c r="Q990" s="1"/>
-      <c r="R990" s="1"/>
-      <c r="S990" s="1"/>
-      <c r="T990" s="1"/>
-      <c r="U990" s="1"/>
-      <c r="V990" s="1"/>
-    </row>
-    <row r="991" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A991" s="1"/>
-      <c r="B991" s="1"/>
-      <c r="G991" s="1"/>
-      <c r="H991" s="1"/>
-      <c r="I991" s="1"/>
-      <c r="J991" s="1"/>
-      <c r="K991" s="1"/>
-      <c r="L991" s="1"/>
-      <c r="M991" s="1"/>
-      <c r="N991" s="1"/>
-      <c r="O991" s="1"/>
-      <c r="P991" s="1"/>
-      <c r="Q991" s="1"/>
-      <c r="R991" s="1"/>
-      <c r="S991" s="1"/>
-      <c r="T991" s="1"/>
-      <c r="U991" s="1"/>
-      <c r="V991" s="1"/>
-    </row>
-    <row r="992" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A992" s="1"/>
-      <c r="B992" s="1"/>
-      <c r="G992" s="1"/>
-      <c r="H992" s="1"/>
-      <c r="I992" s="1"/>
-      <c r="J992" s="1"/>
-      <c r="K992" s="1"/>
-      <c r="L992" s="1"/>
-      <c r="M992" s="1"/>
-      <c r="N992" s="1"/>
-      <c r="O992" s="1"/>
-      <c r="P992" s="1"/>
-      <c r="Q992" s="1"/>
-      <c r="R992" s="1"/>
-      <c r="S992" s="1"/>
-      <c r="T992" s="1"/>
-      <c r="U992" s="1"/>
-      <c r="V992" s="1"/>
-    </row>
-    <row r="993" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A993" s="1"/>
-      <c r="B993" s="1"/>
-      <c r="I993" s="1"/>
-      <c r="J993" s="1"/>
-      <c r="K993" s="1"/>
-      <c r="L993" s="1"/>
-      <c r="M993" s="1"/>
-      <c r="N993" s="1"/>
-      <c r="O993" s="1"/>
-      <c r="P993" s="1"/>
-      <c r="Q993" s="1"/>
-      <c r="R993" s="1"/>
-      <c r="S993" s="1"/>
-      <c r="T993" s="1"/>
-      <c r="U993" s="1"/>
-      <c r="V993" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Faz query Raven data e conta_aglutinada
</commit_message>
<xml_diff>
--- a/arquivo_linkado.xlsx
+++ b/arquivo_linkado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Magal\Desktop\NEW_SAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C8D678-C599-40BC-B8DB-35BB1617E0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42078E85-F6CC-4AE2-89E4-B4C5B5E5B8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="135">
   <si>
     <t>Coluna extraída</t>
   </si>
@@ -443,7 +443,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +464,35 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -493,12 +522,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,8 +751,8 @@
   <dimension ref="A1:V937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2899,7 +2933,9 @@
       <c r="V58" s="1"/>
     </row>
     <row r="59" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+      <c r="A59" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="B59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -2919,7 +2955,9 @@
       <c r="V59" s="1"/>
     </row>
     <row r="60" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+      <c r="A60" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="B60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -2939,7 +2977,9 @@
       <c r="V60" s="1"/>
     </row>
     <row r="61" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+      <c r="A61" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="B61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -2959,7 +2999,9 @@
       <c r="V61" s="1"/>
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+      <c r="A62" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="B62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -2979,7 +3021,9 @@
       <c r="V62" s="1"/>
     </row>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
+      <c r="A63" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="B63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -2999,7 +3043,9 @@
       <c r="V63" s="1"/>
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+      <c r="A64" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="B64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -3019,7 +3065,9 @@
       <c r="V64" s="1"/>
     </row>
     <row r="65" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+      <c r="A65" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="B65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -3039,7 +3087,9 @@
       <c r="V65" s="1"/>
     </row>
     <row r="66" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
+      <c r="A66" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="B66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -3059,7 +3109,9 @@
       <c r="V66" s="1"/>
     </row>
     <row r="67" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A67" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="B67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -3079,7 +3131,9 @@
       <c r="V67" s="1"/>
     </row>
     <row r="68" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+      <c r="A68" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="B68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -3099,7 +3153,9 @@
       <c r="V68" s="1"/>
     </row>
     <row r="69" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
+      <c r="A69" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="B69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3119,7 +3175,9 @@
       <c r="V69" s="1"/>
     </row>
     <row r="70" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
+      <c r="A70" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="B70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3139,7 +3197,9 @@
       <c r="V70" s="1"/>
     </row>
     <row r="71" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
+      <c r="A71" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="B71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -3159,7 +3219,9 @@
       <c r="V71" s="1"/>
     </row>
     <row r="72" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
+      <c r="A72" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="B72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -3179,7 +3241,9 @@
       <c r="V72" s="1"/>
     </row>
     <row r="73" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
+      <c r="A73" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="B73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
@@ -3199,7 +3263,9 @@
       <c r="V73" s="1"/>
     </row>
     <row r="74" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+      <c r="A74" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="B74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -3219,7 +3285,9 @@
       <c r="V74" s="1"/>
     </row>
     <row r="75" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
+      <c r="A75" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="B75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -3239,7 +3307,9 @@
       <c r="V75" s="1"/>
     </row>
     <row r="76" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="A76" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="B76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -3259,7 +3329,9 @@
       <c r="V76" s="1"/>
     </row>
     <row r="77" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="B77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -3279,7 +3351,6 @@
       <c r="V77" s="1"/>
     </row>
     <row r="78" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -3299,7 +3370,6 @@
       <c r="V78" s="1"/>
     </row>
     <row r="79" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -3319,7 +3389,6 @@
       <c r="V79" s="1"/>
     </row>
     <row r="80" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -3338,8 +3407,7 @@
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
     </row>
-    <row r="81" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+    <row r="81" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -3358,8 +3426,7 @@
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
     </row>
-    <row r="82" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
+    <row r="82" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
@@ -3378,8 +3445,7 @@
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
     </row>
-    <row r="83" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
+    <row r="83" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -3398,8 +3464,7 @@
       <c r="U83" s="1"/>
       <c r="V83" s="1"/>
     </row>
-    <row r="84" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+    <row r="84" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -3418,8 +3483,7 @@
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
     </row>
-    <row r="85" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+    <row r="85" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -3438,8 +3502,7 @@
       <c r="U85" s="1"/>
       <c r="V85" s="1"/>
     </row>
-    <row r="86" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+    <row r="86" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -3458,8 +3521,7 @@
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
     </row>
-    <row r="87" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+    <row r="87" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
@@ -3478,8 +3540,7 @@
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
     </row>
-    <row r="88" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
+    <row r="88" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -3498,8 +3559,7 @@
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
     </row>
-    <row r="89" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
+    <row r="89" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -3518,8 +3578,7 @@
       <c r="U89" s="1"/>
       <c r="V89" s="1"/>
     </row>
-    <row r="90" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
+    <row r="90" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -3538,8 +3597,7 @@
       <c r="U90" s="1"/>
       <c r="V90" s="1"/>
     </row>
-    <row r="91" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+    <row r="91" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -3558,8 +3616,7 @@
       <c r="U91" s="1"/>
       <c r="V91" s="1"/>
     </row>
-    <row r="92" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
+    <row r="92" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -3578,8 +3635,7 @@
       <c r="U92" s="1"/>
       <c r="V92" s="1"/>
     </row>
-    <row r="93" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
+    <row r="93" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
@@ -3598,8 +3654,7 @@
       <c r="U93" s="1"/>
       <c r="V93" s="1"/>
     </row>
-    <row r="94" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
+    <row r="94" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
@@ -3618,8 +3673,7 @@
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
     </row>
-    <row r="95" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
+    <row r="95" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -3638,8 +3692,7 @@
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
     </row>
-    <row r="96" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
+    <row r="96" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -3659,7 +3712,6 @@
       <c r="V96" s="1"/>
     </row>
     <row r="97" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>

</xml_diff>